<commit_message>
update input data xlsx
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/02_input_prepared/Maersk_Example_Input_prepared.xlsx
+++ b/spine_projects/01_input_data/02_input_prepared/Maersk_Example_Input_prepared.xlsx
@@ -519,7 +519,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -531,7 +531,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -567,7 +567,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -579,7 +579,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -591,7 +591,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -615,7 +615,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -627,7 +627,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -639,7 +639,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -651,7 +651,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1349,7 +1349,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1359,18 +1359,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1414,7 +1416,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1427,9 +1429,15 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
       <c r="G5" t="n">
         <v>100000</v>
       </c>
@@ -1437,7 +1445,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1447,7 +1455,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -1458,7 +1466,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1471,23 +1479,15 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>100000</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1497,13 +1497,21 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+          <t>balance_type_node</t>
+        </is>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1529,7 +1537,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1539,20 +1547,18 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1565,15 +1571,9 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>100000</v>
       </c>
@@ -1581,7 +1581,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1604,7 +1604,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1739,7 +1739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1778,21 +1778,11 @@
           <t>value</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>fom_cost</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>vom_cost</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1818,10 +1808,6 @@
       <c r="F2" t="n">
         <v>304</v>
       </c>
-      <c r="G2" t="n">
-        <v>100</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1852,13 +1838,11 @@
       <c r="F3" t="n">
         <v>52</v>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1873,13 +1857,15 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
+          <t>Power_Kasso</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>vom_cost</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1901,18 +1887,16 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1927,13 +1911,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1948,23 +1930,21 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CO2_Vaporizer</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1979,19 +1959,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>unit_capacity</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>100</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+          <t>Carbon_Dioxide</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2006,23 +1978,27 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Destilation_Tower</t>
+          <t>CO2_Vaporizer</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+          <t>Vaporized_Carbon_Dioxide</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>unit_capacity</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2037,19 +2013,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>unit_capacity</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>52</v>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+          <t>Raw_Methanol</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2064,23 +2032,27 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Destilation_Tower</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+          <t>E-Methanol_Kasso</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>unit_capacity</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2095,19 +2067,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>unit_capacity</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>100</v>
-      </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+          <t>Hydrogen_Kasso</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2127,18 +2091,22 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+          <t>Raw_Methanol</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>unit_capacity</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>unit__to_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2153,56 +2121,46 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>unit_capacity</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>100</v>
-      </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+          <t>Vaporized_Carbon_Dioxide</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>unit__from_node</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>connection_capacity</t>
+          <t>unit_capacity</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2217,7 +2175,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2228,15 +2186,11 @@
       <c r="F16" t="n">
         <v>1000</v>
       </c>
-      <c r="G16" t="n">
-        <v>100</v>
-      </c>
-      <c r="H16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2262,13 +2216,11 @@
       <c r="F17" t="n">
         <v>1000</v>
       </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2283,7 +2235,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2294,13 +2246,11 @@
       <c r="F18" t="n">
         <v>1000</v>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>connection__from_node</t>
+          <t>connection__to_node</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2310,23 +2260,27 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+          <t>Power_Wholesale</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>connection__to_node</t>
+          <t>connection__from_node</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2341,21 +2295,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="n">
-        <v>1</v>
-      </c>
+          <t>Hydrogen_Kasso</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2375,19 +2319,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>connection_capacity</t>
+          <t>vom_cost</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2407,13 +2349,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+          <t>Hydrogen_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2428,18 +2374,22 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+          <t>Hydrogen_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2454,24 +2404,16 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+          <t>Hydrogen_Kasso</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2491,19 +2433,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>connection_capacity</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+          <t>E-Methanol_Kasso</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2523,13 +2457,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+          <t>E-Methanol_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2544,12 +2482,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2560,8 +2498,6 @@
       <c r="F27" t="n">
         <v>1000</v>
       </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2576,24 +2512,76 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>pipeline_storage_e-methanol</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>E-Methanol_Kasso</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>connection__from_node</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>pipeline_District_Heating</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Waste_Heat</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>connection_capacity</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>connection__to_node</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>pipeline_District_Heating</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
         <is>
           <t>District_Heating</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>connection_capacity</t>
         </is>
       </c>
-      <c r="F28" t="n">
+      <c r="F30" t="n">
         <v>1000</v>
       </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix bug in connection out in relation
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/02_input_prepared/Maersk_Example_Input_prepared.xlsx
+++ b/spine_projects/01_input_data/02_input_prepared/Maersk_Example_Input_prepared.xlsx
@@ -851,7 +851,7 @@
         <v>-28.32</v>
       </c>
       <c r="D6" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -867,7 +867,7 @@
         <v>-10.07</v>
       </c>
       <c r="D7" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -883,7 +883,7 @@
         <v>4.08</v>
       </c>
       <c r="D8" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -899,7 +899,7 @@
         <v>9.91</v>
       </c>
       <c r="D9" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -915,7 +915,7 @@
         <v>7.41</v>
       </c>
       <c r="D10" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -931,7 +931,7 @@
         <v>12.55</v>
       </c>
       <c r="D11" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -947,7 +947,7 @@
         <v>17.25</v>
       </c>
       <c r="D12" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -963,7 +963,7 @@
         <v>15.07</v>
       </c>
       <c r="D13" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -979,7 +979,7 @@
         <v>4.93</v>
       </c>
       <c r="D14" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -995,7 +995,7 @@
         <v>6.33</v>
       </c>
       <c r="D15" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1011,7 +1011,7 @@
         <v>4.93</v>
       </c>
       <c r="D16" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1027,7 +1027,7 @@
         <v>-0.45</v>
       </c>
       <c r="D17" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1043,7 +1043,7 @@
         <v>-0.12</v>
       </c>
       <c r="D18" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1059,7 +1059,7 @@
         <v>0.02</v>
       </c>
       <c r="D19" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1075,7 +1075,7 @@
         <v>-0</v>
       </c>
       <c r="D20" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1091,7 +1091,7 @@
         <v>0.03</v>
       </c>
       <c r="D21" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1107,7 +1107,7 @@
         <v>-1.97</v>
       </c>
       <c r="D22" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1123,7 +1123,7 @@
         <v>-9.06</v>
       </c>
       <c r="D23" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1139,7 +1139,7 @@
         <v>-0.07000000000000001</v>
       </c>
       <c r="D24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1155,7 +1155,7 @@
         <v>4.97</v>
       </c>
       <c r="D25" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1171,7 +1171,7 @@
         <v>6.98</v>
       </c>
       <c r="D26" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1187,7 +1187,7 @@
         <v>16.01</v>
       </c>
       <c r="D27" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1203,7 +1203,7 @@
         <v>4.87</v>
       </c>
       <c r="D28" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1219,7 +1219,7 @@
         <v>28.93</v>
       </c>
       <c r="D29" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1235,7 +1235,7 @@
         <v>33.57</v>
       </c>
       <c r="D30" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1251,7 +1251,7 @@
         <v>45.919998</v>
       </c>
       <c r="D31" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1267,7 +1267,7 @@
         <v>48.290001</v>
       </c>
       <c r="D32" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1283,7 +1283,7 @@
         <v>33.599998</v>
       </c>
       <c r="D33" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1299,7 +1299,7 @@
         <v>33.540001</v>
       </c>
       <c r="D34" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1315,7 +1315,7 @@
         <v>17.790001</v>
       </c>
       <c r="D35" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1331,7 +1331,7 @@
         <v>0.01</v>
       </c>
       <c r="D36" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1347,7 +1347,7 @@
         <v>-37.43</v>
       </c>
       <c r="D37" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1363,7 +1363,7 @@
         <v>-48.060001</v>
       </c>
       <c r="D38" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1379,7 +1379,7 @@
         <v>-50.740002</v>
       </c>
       <c r="D39" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1395,7 +1395,7 @@
         <v>-48.110001</v>
       </c>
       <c r="D40" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1411,7 +1411,7 @@
         <v>-48.66</v>
       </c>
       <c r="D41" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1427,7 +1427,7 @@
         <v>-49.939999</v>
       </c>
       <c r="D42" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1443,7 +1443,7 @@
         <v>-47.259998</v>
       </c>
       <c r="D43" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1459,7 +1459,7 @@
         <v>-49.639999</v>
       </c>
       <c r="D44" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1475,7 +1475,7 @@
         <v>-53.669998</v>
       </c>
       <c r="D45" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1491,7 +1491,7 @@
         <v>-56.009998</v>
       </c>
       <c r="D46" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1507,7 +1507,7 @@
         <v>-56.950001</v>
       </c>
       <c r="D47" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1523,7 +1523,7 @@
         <v>-55.389999</v>
       </c>
       <c r="D48" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1539,7 +1539,7 @@
         <v>-54.900002</v>
       </c>
       <c r="D49" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1555,7 +1555,7 @@
         <v>-53.860001</v>
       </c>
       <c r="D50" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1571,7 +1571,7 @@
         <v>-52.709999</v>
       </c>
       <c r="D51" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1587,7 +1587,7 @@
         <v>-52.09</v>
       </c>
       <c r="D52" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1603,7 +1603,7 @@
         <v>-50.759998</v>
       </c>
       <c r="D53" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3803,7 +3803,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4036,12 +4036,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Methanol_Reactor</t>
+          <t>Electrolyzer</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -4055,42 +4055,42 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>connection__node__node</t>
+          <t>unit__node__node</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>Methanol_Reactor</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>fix_ratio_out_in_connection_flow</t>
+          <t>fix_ratio_out_out_unit_flow</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -4106,17 +4106,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>power_line_Wholesale_Kasso</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -4141,17 +4141,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -4176,17 +4176,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -4211,25 +4211,95 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>pipeline_District_Heating</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>District_Heating</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Waste_Heat</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>fix_ratio_out_in_connection_flow</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>connection__node__node</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>pipeline_storage_hydrogen</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Hydrogen_Kasso</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Hydrogen_storage_Kasso</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>fix_ratio_out_in_connection_flow</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>connection__node__node</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>connection</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>E-Methanol_Kasso</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>fix_ratio_out_in_connection_flow</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="G14" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added fom costs to definition
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/02_input_prepared/Maersk_Example_Input_prepared.xlsx
+++ b/spine_projects/01_input_data/02_input_prepared/Maersk_Example_Input_prepared.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
           <t>Category</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>fom_cost</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -468,6 +473,9 @@
           <t>unit</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -480,6 +488,7 @@
           <t>unit</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -492,6 +501,7 @@
           <t>unit</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -504,6 +514,7 @@
           <t>unit</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -516,11 +527,12 @@
           <t>unit</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -528,11 +540,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -540,11 +553,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -552,11 +566,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -564,6 +579,7 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -576,11 +592,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -588,11 +605,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -600,11 +618,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -612,11 +631,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -624,11 +644,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -636,11 +657,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -648,11 +670,12 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -660,6 +683,7 @@
           <t>node</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -672,6 +696,9 @@
           <t>connection</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -684,6 +711,7 @@
           <t>connection</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -696,6 +724,7 @@
           <t>connection</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -708,6 +737,7 @@
           <t>connection</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2199,7 +2229,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2220,25 +2250,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>fom_cost</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>balance_type</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>has_state</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>node_state_cap</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>frac_state_loss</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>node_slack_penalty</t>
         </is>
@@ -2247,7 +2282,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2255,20 +2290,23 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>balance_type_node</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2276,28 +2314,23 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
         <is>
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
         <v>100000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2305,20 +2338,29 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
         <is>
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2326,15 +2368,18 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>balance_type_node</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2347,22 +2392,23 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
         <is>
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
         <v>100000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2370,20 +2416,21 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
         <is>
           <t>balance_type_none</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2391,22 +2438,21 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>balance_type_none</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2414,22 +2460,21 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
         <is>
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2437,22 +2482,21 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>balance_type_none</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2460,22 +2504,29 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
         <is>
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>100000</v>
+      </c>
       <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
         <v>100000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2483,20 +2534,21 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
         <is>
           <t>balance_type_none</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2504,21 +2556,16 @@
           <t>node</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
         <is>
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="n">
         <v>100000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update data prep for variable efficiency
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/02_input_prepared/Maersk_Example_Input_prepared.xlsx
+++ b/spine_projects/01_input_data/02_input_prepared/Maersk_Example_Input_prepared.xlsx
@@ -532,7 +532,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -545,7 +545,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -571,7 +571,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -584,7 +584,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -597,7 +597,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -610,7 +610,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -623,7 +623,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -636,7 +636,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -649,7 +649,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -662,7 +662,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -675,7 +675,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2277,7 +2277,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Power_Kasso</t>
+          <t>Water</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2287,20 +2287,18 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E-Methanol_Kasso</t>
+          <t>Vaporized_Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2323,7 +2321,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E-Methanol_storage_Kasso</t>
+          <t>Carbon_Dioxide</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2333,28 +2331,18 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>100000</v>
-      </c>
+          <t>balance_type_none</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Vaporized_Carbon_Dioxide</t>
+          <t>Waste_Heat</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2370,14 +2358,12 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Waste_Heat</t>
+          <t>E-Methanol_Kasso</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2393,12 +2379,14 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Carbon_Dioxide</t>
+          <t>Power_Wholesale</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2419,7 +2407,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hydrogen_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2432,9 +2420,17 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
       <c r="G8" t="n">
         <v>100000</v>
       </c>
@@ -2442,7 +2438,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Raw_Methanol</t>
+          <t>District_Heating</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2452,20 +2448,18 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>balance_type_node</t>
+          <t>balance_type_none</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="n">
-        <v>100000</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>District_Heating</t>
+          <t>Hydrogen_Kasso</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2475,18 +2469,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Water</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2496,18 +2492,28 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+          <t>balance_type_node</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>Power_Kasso</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2520,17 +2526,9 @@
           <t>balance_type_node</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>100000</v>
       </c>
@@ -2538,7 +2536,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Power_Wholesale</t>
+          <t>Raw_Methanol</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2548,13 +2546,15 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>balance_type_none</t>
+          <t>balance_type_node</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>100000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3306,7 +3306,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3854,6 +3854,36 @@
       </c>
       <c r="F18" t="n">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>unit__to_node</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Electrolyzer</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Hydrogen_Kasso</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>ordered_unit_flow_op</t>
+        </is>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>